<commit_message>
Categorize temperatures and data summary
</commit_message>
<xml_diff>
--- a/electrophysiology/data/neurophys_lab_sample_data/temperature_dataset.xlsx
+++ b/electrophysiology/data/neurophys_lab_sample_data/temperature_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fau-my.sharepoint.com/personal/thindle2016_fau_edu/Documents/GitHub/laboratory-workshops/electrophysiology/data/neurophys_lab_sample_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thindle2016\OneDrive - Florida Atlantic University\GitHub\laboratory-workshops\electrophysiology\data\neurophys_lab_sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{67091E2F-16EB-B94A-9C62-CFFFF351CDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0337347F-7544-C744-9018-EC9C416C05C8}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{67091E2F-16EB-B94A-9C62-CFFFF351CDAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BCF14DD-D912-4544-A1FB-3B37CE33AB13}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-1980" windowWidth="38400" windowHeight="21100" xr2:uid="{197ADEE1-4E7E-B04C-B2B2-9506562FBAB0}"/>
+    <workbookView xWindow="29400" yWindow="-1980" windowWidth="38400" windowHeight="21105" xr2:uid="{197ADEE1-4E7E-B04C-B2B2-9506562FBAB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -130,6 +119,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59005201-1FD1-4841-81E1-EF34D47010DC}" name="Table1" displayName="Table1" ref="A1:I19" totalsRowShown="0">
+  <autoFilter ref="A1:I19" xr:uid="{A3E753BA-DBA9-46A3-96E8-5231FA712BE2}"/>
+  <sortState ref="A2:I19">
+    <sortCondition ref="C1:C19"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{51B74560-2CFD-4B63-826E-8F1584DCEEF5}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{4099B13D-E504-4171-9108-22B120E55B41}" name="Axon"/>
+    <tableColumn id="3" xr3:uid="{6841FA3E-5014-4B53-969E-91B7D85520C1}" name="Temp (deg C)"/>
+    <tableColumn id="4" xr3:uid="{1E355DF3-2EC3-44ED-91C6-AA12751713BE}" name="L-G1 (mm)"/>
+    <tableColumn id="5" xr3:uid="{80007870-6F01-4356-8D9F-54D4C697575C}" name="L-G1 (ms)"/>
+    <tableColumn id="6" xr3:uid="{3EC3916E-D423-423B-9650-AC19DD6D6CE5}" name="L-G2 (mm)"/>
+    <tableColumn id="7" xr3:uid="{4E177EFC-8F3D-43C9-AB40-7611F2CFEFBE}" name="L-G2 (ms)"/>
+    <tableColumn id="8" xr3:uid="{14D0B762-29FB-4FEE-8701-B29675A718A3}" name="G1-G2 (mm)"/>
+    <tableColumn id="9" xr3:uid="{A205FAC0-4E39-47B7-8AF6-2E4B710FC270}" name="G1-G2 (ms)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,21 +441,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1A95D0-DE6E-9540-8CA4-CC029C87E3F9}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="213" zoomScaleNormal="213" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.625" customWidth="1"/>
+    <col min="3" max="3" width="12.25" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,65 +486,65 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2">
-        <v>21.6</v>
+        <v>12.8</v>
       </c>
       <c r="D2">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>3.6720000000000002</v>
+        <v>6.976</v>
       </c>
       <c r="F2">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="G2">
-        <v>4.4509999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="H2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I2">
-        <v>0.83450000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.0049999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>18</v>
+        <v>13.1</v>
       </c>
       <c r="D3">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="E3">
-        <v>4.5190000000000001</v>
+        <v>15.75</v>
       </c>
       <c r="F3">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="G3">
-        <v>5.4880000000000004</v>
+        <v>17.14</v>
       </c>
       <c r="H3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I3">
-        <v>1.1839999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.478</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -561,7 +573,7 @@
         <v>1.022</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -569,202 +581,202 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>21.6</v>
+        <v>14.7</v>
       </c>
       <c r="D5">
         <v>70</v>
       </c>
       <c r="E5">
-        <v>9.3469999999999995</v>
+        <v>9.5760000000000005</v>
       </c>
       <c r="F5">
         <v>80</v>
       </c>
       <c r="G5">
-        <v>10.46</v>
+        <v>11.41</v>
       </c>
       <c r="H5">
         <v>15</v>
       </c>
       <c r="I5">
-        <v>1.28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.722</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>18.2</v>
+        <v>15.7</v>
       </c>
       <c r="D6">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="E6">
-        <v>10.11</v>
+        <v>11.24</v>
       </c>
       <c r="F6">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="G6">
-        <v>12.05</v>
+        <v>12.99</v>
       </c>
       <c r="H6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I6">
-        <v>1.883</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.591</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>14.7</v>
+        <v>15.7</v>
       </c>
       <c r="D7">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="E7">
-        <v>9.5760000000000005</v>
+        <v>4.7729999999999997</v>
       </c>
       <c r="F7">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="G7">
-        <v>11.41</v>
+        <v>5.8869999999999996</v>
       </c>
       <c r="H7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I7">
-        <v>1.722</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>21.9</v>
+        <v>17.3</v>
       </c>
       <c r="D8">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E8">
-        <v>3.6070000000000002</v>
+        <v>6.976</v>
       </c>
       <c r="F8">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="G8">
-        <v>4.2960000000000003</v>
+        <v>7.7450000000000001</v>
       </c>
       <c r="H8">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I8">
-        <v>0.63649999999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.82769999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>18.2</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="D9">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E9">
-        <v>5.3570000000000002</v>
+        <v>15.43</v>
       </c>
       <c r="F9">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="G9">
-        <v>6.63</v>
+        <v>16.91</v>
       </c>
       <c r="H9">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I9">
-        <v>1.2729999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.655</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10">
-        <v>15.7</v>
+        <v>18</v>
       </c>
       <c r="D10">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="E10">
-        <v>4.7729999999999997</v>
+        <v>4.5190000000000001</v>
       </c>
       <c r="F10">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="G10">
-        <v>5.8869999999999996</v>
+        <v>5.4880000000000004</v>
       </c>
       <c r="H10">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I10">
-        <v>1.008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.1839999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11">
-        <v>21.9</v>
+        <v>18.2</v>
       </c>
       <c r="D11">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="E11">
-        <v>6.5570000000000004</v>
+        <v>10.11</v>
       </c>
       <c r="F11">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="G11">
-        <v>7.2130000000000001</v>
+        <v>12.05</v>
       </c>
       <c r="H11">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11">
-        <v>0.74250000000000005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.883</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -793,152 +805,152 @@
         <v>1.6439999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>15.7</v>
+        <v>18.2</v>
       </c>
       <c r="D13">
         <v>95</v>
       </c>
       <c r="E13">
-        <v>11.24</v>
+        <v>5.3570000000000002</v>
       </c>
       <c r="F13">
         <v>115</v>
       </c>
       <c r="G13">
-        <v>12.99</v>
+        <v>6.63</v>
       </c>
       <c r="H13">
         <v>16</v>
       </c>
       <c r="I13">
-        <v>1.591</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.2729999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>22.8</v>
+        <v>21.6</v>
       </c>
       <c r="D14">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E14">
-        <v>5.2619999999999996</v>
+        <v>9.3469999999999995</v>
       </c>
       <c r="F14">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="G14">
-        <v>5.9710000000000001</v>
+        <v>10.46</v>
       </c>
       <c r="H14">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I14">
-        <v>0.70940000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15">
-        <v>17.3</v>
+        <v>21.6</v>
       </c>
       <c r="D15">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E15">
-        <v>6.976</v>
+        <v>3.6720000000000002</v>
       </c>
       <c r="F15">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="G15">
-        <v>7.7450000000000001</v>
+        <v>4.4509999999999996</v>
       </c>
       <c r="H15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I15">
-        <v>0.82769999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.83450000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>21.9</v>
+      </c>
+      <c r="D16">
+        <v>95</v>
+      </c>
+      <c r="E16">
+        <v>6.5570000000000004</v>
+      </c>
+      <c r="F16">
+        <v>115</v>
+      </c>
+      <c r="G16">
+        <v>7.2130000000000001</v>
+      </c>
+      <c r="H16">
+        <v>16</v>
+      </c>
+      <c r="I16">
+        <v>0.74250000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
         <v>3</v>
       </c>
-      <c r="C16">
-        <v>12.8</v>
-      </c>
-      <c r="D16">
-        <v>100</v>
-      </c>
-      <c r="E16">
-        <v>6.976</v>
-      </c>
-      <c r="F16">
-        <v>105</v>
-      </c>
-      <c r="G16">
-        <v>8.1</v>
-      </c>
-      <c r="H16">
-        <v>10</v>
-      </c>
-      <c r="I16">
-        <v>1.0049999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
       <c r="C17">
-        <v>2.5</v>
+        <v>21.9</v>
       </c>
       <c r="D17">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E17">
-        <v>8.8089999999999993</v>
+        <v>3.6070000000000002</v>
       </c>
       <c r="F17">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="G17">
-        <v>9.5180000000000007</v>
+        <v>4.2960000000000003</v>
       </c>
       <c r="H17">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I17">
-        <v>0.65029999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.63649999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -946,57 +958,60 @@
         <v>4</v>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>22.8</v>
       </c>
       <c r="D18">
         <v>100</v>
       </c>
       <c r="E18">
-        <v>15.43</v>
+        <v>8.8089999999999993</v>
       </c>
       <c r="F18">
         <v>105</v>
       </c>
       <c r="G18">
-        <v>16.91</v>
+        <v>9.5180000000000007</v>
       </c>
       <c r="H18">
         <v>10</v>
       </c>
       <c r="I18">
-        <v>1.655</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.65029999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>22.8</v>
       </c>
       <c r="D19">
         <v>100</v>
       </c>
       <c r="E19">
-        <v>15.75</v>
+        <v>5.2619999999999996</v>
       </c>
       <c r="F19">
         <v>105</v>
       </c>
       <c r="G19">
-        <v>17.14</v>
+        <v>5.9710000000000001</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19">
-        <v>1.478</v>
+        <v>0.70940000000000003</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>